<commit_message>
Added forecast data for test 2
Produced all relevant graphs and added all relevant data with uncertainties in xlsx file
</commit_message>
<xml_diff>
--- a/sales_data.xlsx
+++ b/sales_data.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\TheEntertainer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikos\Desktop\itim\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="22860" windowHeight="9090" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="6" r:id="rId1"/>
@@ -1745,13 +1745,13 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.7265625" style="2"/>
-    <col min="3" max="3" width="87.7265625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="2"/>
+    <col min="3" max="3" width="87.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>441</v>
       </c>
@@ -1759,7 +1759,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
         <v>442</v>
       </c>
@@ -1767,7 +1767,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>443</v>
       </c>
@@ -1785,21 +1785,21 @@
   <dimension ref="A1:DE165"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="4" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="4" topLeftCell="D10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="DD15" sqref="DD15"/>
+      <selection pane="bottomRight" activeCell="B168" sqref="B168"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="107" width="8.7265625" style="1"/>
-    <col min="109" max="109" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="107" width="8.7109375" style="1"/>
+    <col min="109" max="109" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>439</v>
       </c>
@@ -1807,7 +1807,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="2" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:109" x14ac:dyDescent="0.25">
       <c r="D2" s="1" t="s">
         <v>331</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="3" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:109" x14ac:dyDescent="0.25">
       <c r="D3" s="1">
         <v>2014</v>
       </c>
@@ -2435,7 +2435,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="4" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>435</v>
       </c>
@@ -2764,7 +2764,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="5" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
@@ -3087,15 +3087,15 @@
         <v>244</v>
       </c>
       <c r="DD5">
-        <f>SUM(D5:DC5)</f>
+        <f t="shared" ref="DD5:DD36" si="0">SUM(D5:DC5)</f>
         <v>43740</v>
       </c>
       <c r="DE5" s="1">
-        <f>COUNT(D5:DC5)</f>
+        <f t="shared" ref="DE5:DE36" si="1">COUNT(D5:DC5)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>54</v>
       </c>
@@ -3418,15 +3418,15 @@
         <v>3005</v>
       </c>
       <c r="DD6">
-        <f>SUM(D6:DC6)</f>
+        <f t="shared" si="0"/>
         <v>198896</v>
       </c>
       <c r="DE6" s="1">
-        <f>COUNT(D6:DC6)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>54</v>
       </c>
@@ -3749,15 +3749,15 @@
         <v>23621</v>
       </c>
       <c r="DD7">
-        <f>SUM(D7:DC7)</f>
+        <f t="shared" si="0"/>
         <v>3474306</v>
       </c>
       <c r="DE7" s="1">
-        <f>COUNT(D7:DC7)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>54</v>
       </c>
@@ -4080,15 +4080,15 @@
         <v>1274</v>
       </c>
       <c r="DD8">
-        <f>SUM(D8:DC8)</f>
+        <f t="shared" si="0"/>
         <v>326277</v>
       </c>
       <c r="DE8" s="1">
-        <f>COUNT(D8:DC8)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>54</v>
       </c>
@@ -4411,15 +4411,15 @@
         <v>9490</v>
       </c>
       <c r="DD9">
-        <f>SUM(D9:DC9)</f>
+        <f t="shared" si="0"/>
         <v>1281094</v>
       </c>
       <c r="DE9" s="1">
-        <f>COUNT(D9:DC9)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>54</v>
       </c>
@@ -4742,15 +4742,15 @@
         <v>0</v>
       </c>
       <c r="DD10">
-        <f>SUM(D10:DC10)</f>
+        <f t="shared" si="0"/>
         <v>139</v>
       </c>
       <c r="DE10" s="1">
-        <f>COUNT(D10:DC10)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -5073,15 +5073,15 @@
         <v>400</v>
       </c>
       <c r="DD11">
-        <f>SUM(D11:DC11)</f>
+        <f t="shared" si="0"/>
         <v>77297</v>
       </c>
       <c r="DE11" s="1">
-        <f>COUNT(D11:DC11)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -5404,15 +5404,15 @@
         <v>527</v>
       </c>
       <c r="DD12">
-        <f>SUM(D12:DC12)</f>
+        <f t="shared" si="0"/>
         <v>339459</v>
       </c>
       <c r="DE12" s="1">
-        <f>COUNT(D12:DC12)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>77</v>
       </c>
@@ -5735,15 +5735,15 @@
         <v>2</v>
       </c>
       <c r="DD13">
-        <f>SUM(D13:DC13)</f>
+        <f t="shared" si="0"/>
         <v>362</v>
       </c>
       <c r="DE13" s="1">
-        <f>COUNT(D13:DC13)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -6066,15 +6066,15 @@
         <v>871</v>
       </c>
       <c r="DD14">
-        <f>SUM(D14:DC14)</f>
+        <f t="shared" si="0"/>
         <v>162284</v>
       </c>
       <c r="DE14" s="1">
-        <f>COUNT(D14:DC14)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -6397,15 +6397,15 @@
         <v>2996</v>
       </c>
       <c r="DD15">
-        <f>SUM(D15:DC15)</f>
+        <f t="shared" si="0"/>
         <v>408966</v>
       </c>
       <c r="DE15" s="1">
-        <f>COUNT(D15:DC15)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>77</v>
       </c>
@@ -6728,15 +6728,15 @@
         <v>6690</v>
       </c>
       <c r="DD16">
-        <f>SUM(D16:DC16)</f>
+        <f t="shared" si="0"/>
         <v>881434</v>
       </c>
       <c r="DE16" s="1">
-        <f>COUNT(D16:DC16)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>77</v>
       </c>
@@ -7059,15 +7059,15 @@
         <v>23980</v>
       </c>
       <c r="DD17">
-        <f>SUM(D17:DC17)</f>
+        <f t="shared" si="0"/>
         <v>8143136</v>
       </c>
       <c r="DE17" s="1">
-        <f>COUNT(D17:DC17)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>77</v>
       </c>
@@ -7390,15 +7390,15 @@
         <v>4966</v>
       </c>
       <c r="DD18">
-        <f>SUM(D18:DC18)</f>
+        <f t="shared" si="0"/>
         <v>913970</v>
       </c>
       <c r="DE18" s="1">
-        <f>COUNT(D18:DC18)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>77</v>
       </c>
@@ -7721,15 +7721,15 @@
         <v>537</v>
       </c>
       <c r="DD19">
-        <f>SUM(D19:DC19)</f>
+        <f t="shared" si="0"/>
         <v>120819</v>
       </c>
       <c r="DE19" s="1">
-        <f>COUNT(D19:DC19)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>77</v>
       </c>
@@ -8052,15 +8052,15 @@
         <v>1056</v>
       </c>
       <c r="DD20">
-        <f>SUM(D20:DC20)</f>
+        <f t="shared" si="0"/>
         <v>317439</v>
       </c>
       <c r="DE20" s="1">
-        <f>COUNT(D20:DC20)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>77</v>
       </c>
@@ -8383,15 +8383,15 @@
         <v>3733</v>
       </c>
       <c r="DD21">
-        <f>SUM(D21:DC21)</f>
+        <f t="shared" si="0"/>
         <v>1124650</v>
       </c>
       <c r="DE21" s="1">
-        <f>COUNT(D21:DC21)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>77</v>
       </c>
@@ -8714,15 +8714,15 @@
         <v>322</v>
       </c>
       <c r="DD22">
-        <f>SUM(D22:DC22)</f>
+        <f t="shared" si="0"/>
         <v>605337</v>
       </c>
       <c r="DE22" s="1">
-        <f>COUNT(D22:DC22)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -9045,15 +9045,15 @@
         <v>8529</v>
       </c>
       <c r="DD23">
-        <f>SUM(D23:DC23)</f>
+        <f t="shared" si="0"/>
         <v>1440361</v>
       </c>
       <c r="DE23" s="1">
-        <f>COUNT(D23:DC23)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>95</v>
       </c>
@@ -9376,15 +9376,15 @@
         <v>8119</v>
       </c>
       <c r="DD24">
-        <f>SUM(D24:DC24)</f>
+        <f t="shared" si="0"/>
         <v>1619508</v>
       </c>
       <c r="DE24" s="1">
-        <f>COUNT(D24:DC24)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -9707,15 +9707,15 @@
         <v>3383</v>
       </c>
       <c r="DD25">
-        <f>SUM(D25:DC25)</f>
+        <f t="shared" si="0"/>
         <v>467775</v>
       </c>
       <c r="DE25" s="1">
-        <f>COUNT(D25:DC25)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -10038,15 +10038,15 @@
         <v>0</v>
       </c>
       <c r="DD26">
-        <f>SUM(D26:DC26)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="DE26" s="1">
-        <f>COUNT(D26:DC26)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>95</v>
       </c>
@@ -10369,15 +10369,15 @@
         <v>0</v>
       </c>
       <c r="DD27">
-        <f>SUM(D27:DC27)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
       <c r="DE27" s="1">
-        <f>COUNT(D27:DC27)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>104</v>
       </c>
@@ -10700,15 +10700,15 @@
         <v>4222</v>
       </c>
       <c r="DD28">
-        <f>SUM(D28:DC28)</f>
+        <f t="shared" si="0"/>
         <v>455147</v>
       </c>
       <c r="DE28" s="1">
-        <f>COUNT(D28:DC28)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>104</v>
       </c>
@@ -11031,15 +11031,15 @@
         <v>10207</v>
       </c>
       <c r="DD29">
-        <f>SUM(D29:DC29)</f>
+        <f t="shared" si="0"/>
         <v>1520058</v>
       </c>
       <c r="DE29" s="1">
-        <f>COUNT(D29:DC29)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>110</v>
       </c>
@@ -11362,15 +11362,15 @@
         <v>2718</v>
       </c>
       <c r="DD30">
-        <f>SUM(D30:DC30)</f>
+        <f t="shared" si="0"/>
         <v>458778</v>
       </c>
       <c r="DE30" s="1">
-        <f>COUNT(D30:DC30)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="31" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -11693,15 +11693,15 @@
         <v>1634</v>
       </c>
       <c r="DD31">
-        <f>SUM(D31:DC31)</f>
+        <f t="shared" si="0"/>
         <v>208535</v>
       </c>
       <c r="DE31" s="1">
-        <f>COUNT(D31:DC31)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="32" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>110</v>
       </c>
@@ -12024,15 +12024,15 @@
         <v>17008</v>
       </c>
       <c r="DD32">
-        <f>SUM(D32:DC32)</f>
+        <f t="shared" si="0"/>
         <v>1772242</v>
       </c>
       <c r="DE32" s="1">
-        <f>COUNT(D32:DC32)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>110</v>
       </c>
@@ -12355,15 +12355,15 @@
         <v>1899</v>
       </c>
       <c r="DD33">
-        <f>SUM(D33:DC33)</f>
+        <f t="shared" si="0"/>
         <v>501998</v>
       </c>
       <c r="DE33" s="1">
-        <f>COUNT(D33:DC33)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="34" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>110</v>
       </c>
@@ -12686,15 +12686,15 @@
         <v>10</v>
       </c>
       <c r="DD34">
-        <f>SUM(D34:DC34)</f>
+        <f t="shared" si="0"/>
         <v>22581</v>
       </c>
       <c r="DE34" s="1">
-        <f>COUNT(D34:DC34)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>110</v>
       </c>
@@ -13017,15 +13017,15 @@
         <v>2</v>
       </c>
       <c r="DD35">
-        <f>SUM(D35:DC35)</f>
+        <f t="shared" si="0"/>
         <v>844</v>
       </c>
       <c r="DE35" s="1">
-        <f>COUNT(D35:DC35)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="36" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>121</v>
       </c>
@@ -13348,15 +13348,15 @@
         <v>0</v>
       </c>
       <c r="DD36">
-        <f>SUM(D36:DC36)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="DE36" s="1">
-        <f>COUNT(D36:DC36)</f>
+        <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="37" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>123</v>
       </c>
@@ -13679,15 +13679,15 @@
         <v>211</v>
       </c>
       <c r="DD37">
-        <f>SUM(D37:DC37)</f>
+        <f t="shared" ref="DD37:DD68" si="2">SUM(D37:DC37)</f>
         <v>12459</v>
       </c>
       <c r="DE37" s="1">
-        <f>COUNT(D37:DC37)</f>
+        <f t="shared" ref="DE37:DE68" si="3">COUNT(D37:DC37)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>123</v>
       </c>
@@ -14010,15 +14010,15 @@
         <v>0</v>
       </c>
       <c r="DD38">
-        <f>SUM(D38:DC38)</f>
+        <f t="shared" si="2"/>
         <v>1246</v>
       </c>
       <c r="DE38" s="1">
-        <f>COUNT(D38:DC38)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="39" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>123</v>
       </c>
@@ -14341,15 +14341,15 @@
         <v>11069</v>
       </c>
       <c r="DD39">
-        <f>SUM(D39:DC39)</f>
+        <f t="shared" si="2"/>
         <v>1120994</v>
       </c>
       <c r="DE39" s="1">
-        <f>COUNT(D39:DC39)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>123</v>
       </c>
@@ -14672,15 +14672,15 @@
         <v>460</v>
       </c>
       <c r="DD40">
-        <f>SUM(D40:DC40)</f>
+        <f t="shared" si="2"/>
         <v>57880</v>
       </c>
       <c r="DE40" s="1">
-        <f>COUNT(D40:DC40)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>123</v>
       </c>
@@ -15003,15 +15003,15 @@
         <v>2845</v>
       </c>
       <c r="DD41">
-        <f>SUM(D41:DC41)</f>
+        <f t="shared" si="2"/>
         <v>542960</v>
       </c>
       <c r="DE41" s="1">
-        <f>COUNT(D41:DC41)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="42" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -15334,15 +15334,15 @@
         <v>673</v>
       </c>
       <c r="DD42">
-        <f>SUM(D42:DC42)</f>
+        <f t="shared" si="2"/>
         <v>156926</v>
       </c>
       <c r="DE42" s="1">
-        <f>COUNT(D42:DC42)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="43" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>123</v>
       </c>
@@ -15665,15 +15665,15 @@
         <v>260</v>
       </c>
       <c r="DD43">
-        <f>SUM(D43:DC43)</f>
+        <f t="shared" si="2"/>
         <v>39290</v>
       </c>
       <c r="DE43" s="1">
-        <f>COUNT(D43:DC43)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="44" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>139</v>
       </c>
@@ -15996,15 +15996,15 @@
         <v>0</v>
       </c>
       <c r="DD44">
-        <f>SUM(D44:DC44)</f>
+        <f t="shared" si="2"/>
         <v>3842</v>
       </c>
       <c r="DE44" s="1">
-        <f>COUNT(D44:DC44)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="45" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>139</v>
       </c>
@@ -16327,15 +16327,15 @@
         <v>0</v>
       </c>
       <c r="DD45">
-        <f>SUM(D45:DC45)</f>
+        <f t="shared" si="2"/>
         <v>43</v>
       </c>
       <c r="DE45" s="1">
-        <f>COUNT(D45:DC45)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="46" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>142</v>
       </c>
@@ -16658,15 +16658,15 @@
         <v>1298</v>
       </c>
       <c r="DD46">
-        <f>SUM(D46:DC46)</f>
+        <f t="shared" si="2"/>
         <v>282836</v>
       </c>
       <c r="DE46" s="1">
-        <f>COUNT(D46:DC46)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="47" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>142</v>
       </c>
@@ -16989,15 +16989,15 @@
         <v>1500</v>
       </c>
       <c r="DD47">
-        <f>SUM(D47:DC47)</f>
+        <f t="shared" si="2"/>
         <v>215362</v>
       </c>
       <c r="DE47" s="1">
-        <f>COUNT(D47:DC47)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>142</v>
       </c>
@@ -17320,15 +17320,15 @@
         <v>5476</v>
       </c>
       <c r="DD48">
-        <f>SUM(D48:DC48)</f>
+        <f t="shared" si="2"/>
         <v>1567151</v>
       </c>
       <c r="DE48" s="1">
-        <f>COUNT(D48:DC48)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>142</v>
       </c>
@@ -17651,15 +17651,15 @@
         <v>111</v>
       </c>
       <c r="DD49">
-        <f>SUM(D49:DC49)</f>
+        <f t="shared" si="2"/>
         <v>40774</v>
       </c>
       <c r="DE49" s="1">
-        <f>COUNT(D49:DC49)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="50" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>142</v>
       </c>
@@ -17982,15 +17982,15 @@
         <v>1620</v>
       </c>
       <c r="DD50">
-        <f>SUM(D50:DC50)</f>
+        <f t="shared" si="2"/>
         <v>537355</v>
       </c>
       <c r="DE50" s="1">
-        <f>COUNT(D50:DC50)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>142</v>
       </c>
@@ -18313,15 +18313,15 @@
         <v>75</v>
       </c>
       <c r="DD51">
-        <f>SUM(D51:DC51)</f>
+        <f t="shared" si="2"/>
         <v>4788</v>
       </c>
       <c r="DE51" s="1">
-        <f>COUNT(D51:DC51)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>142</v>
       </c>
@@ -18644,15 +18644,15 @@
         <v>461</v>
       </c>
       <c r="DD52">
-        <f>SUM(D52:DC52)</f>
+        <f t="shared" si="2"/>
         <v>142387</v>
       </c>
       <c r="DE52" s="1">
-        <f>COUNT(D52:DC52)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>142</v>
       </c>
@@ -18975,15 +18975,15 @@
         <v>555</v>
       </c>
       <c r="DD53">
-        <f>SUM(D53:DC53)</f>
+        <f t="shared" si="2"/>
         <v>125791</v>
       </c>
       <c r="DE53" s="1">
-        <f>COUNT(D53:DC53)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>142</v>
       </c>
@@ -19306,15 +19306,15 @@
         <v>81</v>
       </c>
       <c r="DD54">
-        <f>SUM(D54:DC54)</f>
+        <f t="shared" si="2"/>
         <v>62808</v>
       </c>
       <c r="DE54" s="1">
-        <f>COUNT(D54:DC54)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="55" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>142</v>
       </c>
@@ -19637,15 +19637,15 @@
         <v>0</v>
       </c>
       <c r="DD55">
-        <f>SUM(D55:DC55)</f>
+        <f t="shared" si="2"/>
         <v>61</v>
       </c>
       <c r="DE55" s="1">
-        <f>COUNT(D55:DC55)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>160</v>
       </c>
@@ -19968,15 +19968,15 @@
         <v>20602</v>
       </c>
       <c r="DD56">
-        <f>SUM(D56:DC56)</f>
+        <f t="shared" si="2"/>
         <v>1974423</v>
       </c>
       <c r="DE56" s="1">
-        <f>COUNT(D56:DC56)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="57" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>160</v>
       </c>
@@ -20299,15 +20299,15 @@
         <v>2202</v>
       </c>
       <c r="DD57">
-        <f>SUM(D57:DC57)</f>
+        <f t="shared" si="2"/>
         <v>240144</v>
       </c>
       <c r="DE57" s="1">
-        <f>COUNT(D57:DC57)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="58" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>160</v>
       </c>
@@ -20630,15 +20630,15 @@
         <v>1004</v>
       </c>
       <c r="DD58">
-        <f>SUM(D58:DC58)</f>
+        <f t="shared" si="2"/>
         <v>250636</v>
       </c>
       <c r="DE58" s="1">
-        <f>COUNT(D58:DC58)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="59" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>160</v>
       </c>
@@ -20961,15 +20961,15 @@
         <v>14564</v>
       </c>
       <c r="DD59">
-        <f>SUM(D59:DC59)</f>
+        <f t="shared" si="2"/>
         <v>1452264</v>
       </c>
       <c r="DE59" s="1">
-        <f>COUNT(D59:DC59)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>160</v>
       </c>
@@ -21292,15 +21292,15 @@
         <v>2280</v>
       </c>
       <c r="DD60">
-        <f>SUM(D60:DC60)</f>
+        <f t="shared" si="2"/>
         <v>412417</v>
       </c>
       <c r="DE60" s="1">
-        <f>COUNT(D60:DC60)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>175</v>
       </c>
@@ -21623,15 +21623,15 @@
         <v>0</v>
       </c>
       <c r="DD61">
-        <f>SUM(D61:DC61)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="DE61" s="1">
-        <f>COUNT(D61:DC61)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="62" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>175</v>
       </c>
@@ -21954,15 +21954,15 @@
         <v>1</v>
       </c>
       <c r="DD62">
-        <f>SUM(D62:DC62)</f>
+        <f t="shared" si="2"/>
         <v>4416</v>
       </c>
       <c r="DE62" s="1">
-        <f>COUNT(D62:DC62)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="63" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>175</v>
       </c>
@@ -22285,15 +22285,15 @@
         <v>0</v>
       </c>
       <c r="DD63">
-        <f>SUM(D63:DC63)</f>
+        <f t="shared" si="2"/>
         <v>220</v>
       </c>
       <c r="DE63" s="1">
-        <f>COUNT(D63:DC63)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="64" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>175</v>
       </c>
@@ -22616,15 +22616,15 @@
         <v>1</v>
       </c>
       <c r="DD64">
-        <f>SUM(D64:DC64)</f>
+        <f t="shared" si="2"/>
         <v>6571</v>
       </c>
       <c r="DE64" s="1">
-        <f>COUNT(D64:DC64)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>175</v>
       </c>
@@ -22947,15 +22947,15 @@
         <v>92</v>
       </c>
       <c r="DD65">
-        <f>SUM(D65:DC65)</f>
+        <f t="shared" si="2"/>
         <v>50030</v>
       </c>
       <c r="DE65" s="1">
-        <f>COUNT(D65:DC65)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="66" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>175</v>
       </c>
@@ -23278,15 +23278,15 @@
         <v>212</v>
       </c>
       <c r="DD66">
-        <f>SUM(D66:DC66)</f>
+        <f t="shared" si="2"/>
         <v>99307</v>
       </c>
       <c r="DE66" s="1">
-        <f>COUNT(D66:DC66)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="67" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>175</v>
       </c>
@@ -23609,15 +23609,15 @@
         <v>665</v>
       </c>
       <c r="DD67">
-        <f>SUM(D67:DC67)</f>
+        <f t="shared" si="2"/>
         <v>16409</v>
       </c>
       <c r="DE67" s="1">
-        <f>COUNT(D67:DC67)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="68" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>175</v>
       </c>
@@ -23940,15 +23940,15 @@
         <v>2756</v>
       </c>
       <c r="DD68">
-        <f>SUM(D68:DC68)</f>
+        <f t="shared" si="2"/>
         <v>486806</v>
       </c>
       <c r="DE68" s="1">
-        <f>COUNT(D68:DC68)</f>
+        <f t="shared" si="3"/>
         <v>104</v>
       </c>
     </row>
-    <row r="69" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>175</v>
       </c>
@@ -24271,15 +24271,15 @@
         <v>0</v>
       </c>
       <c r="DD69">
-        <f>SUM(D69:DC69)</f>
+        <f t="shared" ref="DD69:DD100" si="4">SUM(D69:DC69)</f>
         <v>0</v>
       </c>
       <c r="DE69" s="1">
-        <f>COUNT(D69:DC69)</f>
+        <f t="shared" ref="DE69:DE100" si="5">COUNT(D69:DC69)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="70" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>175</v>
       </c>
@@ -24602,15 +24602,15 @@
         <v>0</v>
       </c>
       <c r="DD70">
-        <f>SUM(D70:DC70)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="DE70" s="1">
-        <f>COUNT(D70:DC70)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="71" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>175</v>
       </c>
@@ -24933,15 +24933,15 @@
         <v>69</v>
       </c>
       <c r="DD71">
-        <f>SUM(D71:DC71)</f>
+        <f t="shared" si="4"/>
         <v>29210</v>
       </c>
       <c r="DE71" s="1">
-        <f>COUNT(D71:DC71)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="72" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>175</v>
       </c>
@@ -25264,15 +25264,15 @@
         <v>4702</v>
       </c>
       <c r="DD72">
-        <f>SUM(D72:DC72)</f>
+        <f t="shared" si="4"/>
         <v>682009</v>
       </c>
       <c r="DE72" s="1">
-        <f>COUNT(D72:DC72)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>175</v>
       </c>
@@ -25595,15 +25595,15 @@
         <v>0</v>
       </c>
       <c r="DD73">
-        <f>SUM(D73:DC73)</f>
+        <f t="shared" si="4"/>
         <v>427</v>
       </c>
       <c r="DE73" s="1">
-        <f>COUNT(D73:DC73)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>175</v>
       </c>
@@ -25926,15 +25926,15 @@
         <v>666</v>
       </c>
       <c r="DD74">
-        <f>SUM(D74:DC74)</f>
+        <f t="shared" si="4"/>
         <v>186511</v>
       </c>
       <c r="DE74" s="1">
-        <f>COUNT(D74:DC74)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="75" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>175</v>
       </c>
@@ -26257,15 +26257,15 @@
         <v>3612</v>
       </c>
       <c r="DD75">
-        <f>SUM(D75:DC75)</f>
+        <f t="shared" si="4"/>
         <v>218949</v>
       </c>
       <c r="DE75" s="1">
-        <f>COUNT(D75:DC75)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="76" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>175</v>
       </c>
@@ -26588,15 +26588,15 @@
         <v>39</v>
       </c>
       <c r="DD76">
-        <f>SUM(D76:DC76)</f>
+        <f t="shared" si="4"/>
         <v>20777</v>
       </c>
       <c r="DE76" s="1">
-        <f>COUNT(D76:DC76)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="77" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>175</v>
       </c>
@@ -26919,15 +26919,15 @@
         <v>0</v>
       </c>
       <c r="DD77">
-        <f>SUM(D77:DC77)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="DE77" s="1">
-        <f>COUNT(D77:DC77)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="78" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>175</v>
       </c>
@@ -27250,15 +27250,15 @@
         <v>856</v>
       </c>
       <c r="DD78">
-        <f>SUM(D78:DC78)</f>
+        <f t="shared" si="4"/>
         <v>87151</v>
       </c>
       <c r="DE78" s="1">
-        <f>COUNT(D78:DC78)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="79" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>175</v>
       </c>
@@ -27581,15 +27581,15 @@
         <v>414</v>
       </c>
       <c r="DD79">
-        <f>SUM(D79:DC79)</f>
+        <f t="shared" si="4"/>
         <v>258725</v>
       </c>
       <c r="DE79" s="1">
-        <f>COUNT(D79:DC79)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="80" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>175</v>
       </c>
@@ -27912,15 +27912,15 @@
         <v>494</v>
       </c>
       <c r="DD80">
-        <f>SUM(D80:DC80)</f>
+        <f t="shared" si="4"/>
         <v>118107</v>
       </c>
       <c r="DE80" s="1">
-        <f>COUNT(D80:DC80)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="81" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>175</v>
       </c>
@@ -28243,15 +28243,15 @@
         <v>402</v>
       </c>
       <c r="DD81">
-        <f>SUM(D81:DC81)</f>
+        <f t="shared" si="4"/>
         <v>157674</v>
       </c>
       <c r="DE81" s="1">
-        <f>COUNT(D81:DC81)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>175</v>
       </c>
@@ -28574,15 +28574,15 @@
         <v>65</v>
       </c>
       <c r="DD82">
-        <f>SUM(D82:DC82)</f>
+        <f t="shared" si="4"/>
         <v>25900</v>
       </c>
       <c r="DE82" s="1">
-        <f>COUNT(D82:DC82)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="83" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>175</v>
       </c>
@@ -28905,15 +28905,15 @@
         <v>5677</v>
       </c>
       <c r="DD83">
-        <f>SUM(D83:DC83)</f>
+        <f t="shared" si="4"/>
         <v>744847</v>
       </c>
       <c r="DE83" s="1">
-        <f>COUNT(D83:DC83)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="84" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>175</v>
       </c>
@@ -29236,15 +29236,15 @@
         <v>0</v>
       </c>
       <c r="DD84">
-        <f>SUM(D84:DC84)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="DE84" s="1">
-        <f>COUNT(D84:DC84)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="85" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>175</v>
       </c>
@@ -29567,15 +29567,15 @@
         <v>266</v>
       </c>
       <c r="DD85">
-        <f>SUM(D85:DC85)</f>
+        <f t="shared" si="4"/>
         <v>5979</v>
       </c>
       <c r="DE85" s="1">
-        <f>COUNT(D85:DC85)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="86" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>175</v>
       </c>
@@ -29898,15 +29898,15 @@
         <v>263</v>
       </c>
       <c r="DD86">
-        <f>SUM(D86:DC86)</f>
+        <f t="shared" si="4"/>
         <v>40673</v>
       </c>
       <c r="DE86" s="1">
-        <f>COUNT(D86:DC86)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="87" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>175</v>
       </c>
@@ -30229,15 +30229,15 @@
         <v>1304</v>
       </c>
       <c r="DD87">
-        <f>SUM(D87:DC87)</f>
+        <f t="shared" si="4"/>
         <v>2407</v>
       </c>
       <c r="DE87" s="1">
-        <f>COUNT(D87:DC87)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="88" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>175</v>
       </c>
@@ -30560,15 +30560,15 @@
         <v>3186</v>
       </c>
       <c r="DD88">
-        <f>SUM(D88:DC88)</f>
+        <f t="shared" si="4"/>
         <v>221590</v>
       </c>
       <c r="DE88" s="1">
-        <f>COUNT(D88:DC88)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="89" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>175</v>
       </c>
@@ -30891,15 +30891,15 @@
         <v>0</v>
       </c>
       <c r="DD89">
-        <f>SUM(D89:DC89)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="DE89" s="1">
-        <f>COUNT(D89:DC89)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="90" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>175</v>
       </c>
@@ -31222,15 +31222,15 @@
         <v>56</v>
       </c>
       <c r="DD90">
-        <f>SUM(D90:DC90)</f>
+        <f t="shared" si="4"/>
         <v>9287</v>
       </c>
       <c r="DE90" s="1">
-        <f>COUNT(D90:DC90)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="91" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>175</v>
       </c>
@@ -31553,15 +31553,15 @@
         <v>105</v>
       </c>
       <c r="DD91">
-        <f>SUM(D91:DC91)</f>
+        <f t="shared" si="4"/>
         <v>40000</v>
       </c>
       <c r="DE91" s="1">
-        <f>COUNT(D91:DC91)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="92" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>175</v>
       </c>
@@ -31884,15 +31884,15 @@
         <v>70</v>
       </c>
       <c r="DD92">
-        <f>SUM(D92:DC92)</f>
+        <f t="shared" si="4"/>
         <v>34279</v>
       </c>
       <c r="DE92" s="1">
-        <f>COUNT(D92:DC92)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="93" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>175</v>
       </c>
@@ -32215,15 +32215,15 @@
         <v>0</v>
       </c>
       <c r="DD93">
-        <f>SUM(D93:DC93)</f>
+        <f t="shared" si="4"/>
         <v>312</v>
       </c>
       <c r="DE93" s="1">
-        <f>COUNT(D93:DC93)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="94" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>175</v>
       </c>
@@ -32546,15 +32546,15 @@
         <v>319</v>
       </c>
       <c r="DD94">
-        <f>SUM(D94:DC94)</f>
+        <f t="shared" si="4"/>
         <v>115168</v>
       </c>
       <c r="DE94" s="1">
-        <f>COUNT(D94:DC94)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="95" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>175</v>
       </c>
@@ -32877,15 +32877,15 @@
         <v>0</v>
       </c>
       <c r="DD95">
-        <f>SUM(D95:DC95)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="DE95" s="1">
-        <f>COUNT(D95:DC95)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="96" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>219</v>
       </c>
@@ -33208,15 +33208,15 @@
         <v>1790</v>
       </c>
       <c r="DD96">
-        <f>SUM(D96:DC96)</f>
+        <f t="shared" si="4"/>
         <v>303621</v>
       </c>
       <c r="DE96" s="1">
-        <f>COUNT(D96:DC96)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="97" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>220</v>
       </c>
@@ -33539,15 +33539,15 @@
         <v>319</v>
       </c>
       <c r="DD97">
-        <f>SUM(D97:DC97)</f>
+        <f t="shared" si="4"/>
         <v>94337</v>
       </c>
       <c r="DE97" s="1">
-        <f>COUNT(D97:DC97)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="98" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>220</v>
       </c>
@@ -33870,15 +33870,15 @@
         <v>2</v>
       </c>
       <c r="DD98">
-        <f>SUM(D98:DC98)</f>
+        <f t="shared" si="4"/>
         <v>5111</v>
       </c>
       <c r="DE98" s="1">
-        <f>COUNT(D98:DC98)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="99" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>223</v>
       </c>
@@ -34201,15 +34201,15 @@
         <v>2314</v>
       </c>
       <c r="DD99">
-        <f>SUM(D99:DC99)</f>
+        <f t="shared" si="4"/>
         <v>421942</v>
       </c>
       <c r="DE99" s="1">
-        <f>COUNT(D99:DC99)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="100" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>223</v>
       </c>
@@ -34532,15 +34532,15 @@
         <v>101</v>
       </c>
       <c r="DD100">
-        <f>SUM(D100:DC100)</f>
+        <f t="shared" si="4"/>
         <v>12816</v>
       </c>
       <c r="DE100" s="1">
-        <f>COUNT(D100:DC100)</f>
+        <f t="shared" si="5"/>
         <v>104</v>
       </c>
     </row>
-    <row r="101" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>223</v>
       </c>
@@ -34863,15 +34863,15 @@
         <v>0</v>
       </c>
       <c r="DD101">
-        <f>SUM(D101:DC101)</f>
+        <f t="shared" ref="DD101:DD132" si="6">SUM(D101:DC101)</f>
         <v>2984</v>
       </c>
       <c r="DE101" s="1">
-        <f>COUNT(D101:DC101)</f>
+        <f t="shared" ref="DE101:DE132" si="7">COUNT(D101:DC101)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>223</v>
       </c>
@@ -35194,15 +35194,15 @@
         <v>303</v>
       </c>
       <c r="DD102">
-        <f>SUM(D102:DC102)</f>
+        <f t="shared" si="6"/>
         <v>68847</v>
       </c>
       <c r="DE102" s="1">
-        <f>COUNT(D102:DC102)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="103" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>223</v>
       </c>
@@ -35525,15 +35525,15 @@
         <v>148</v>
       </c>
       <c r="DD103">
-        <f>SUM(D103:DC103)</f>
+        <f t="shared" si="6"/>
         <v>256568</v>
       </c>
       <c r="DE103" s="1">
-        <f>COUNT(D103:DC103)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="104" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>223</v>
       </c>
@@ -35856,15 +35856,15 @@
         <v>2</v>
       </c>
       <c r="DD104">
-        <f>SUM(D104:DC104)</f>
+        <f t="shared" si="6"/>
         <v>858</v>
       </c>
       <c r="DE104" s="1">
-        <f>COUNT(D104:DC104)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="105" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>223</v>
       </c>
@@ -36187,15 +36187,15 @@
         <v>5415</v>
       </c>
       <c r="DD105">
-        <f>SUM(D105:DC105)</f>
+        <f t="shared" si="6"/>
         <v>431228</v>
       </c>
       <c r="DE105" s="1">
-        <f>COUNT(D105:DC105)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="106" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>223</v>
       </c>
@@ -36518,15 +36518,15 @@
         <v>6783</v>
       </c>
       <c r="DD106">
-        <f>SUM(D106:DC106)</f>
+        <f t="shared" si="6"/>
         <v>421612</v>
       </c>
       <c r="DE106" s="1">
-        <f>COUNT(D106:DC106)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="107" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>223</v>
       </c>
@@ -36849,15 +36849,15 @@
         <v>190</v>
       </c>
       <c r="DD107">
-        <f>SUM(D107:DC107)</f>
+        <f t="shared" si="6"/>
         <v>65763</v>
       </c>
       <c r="DE107" s="1">
-        <f>COUNT(D107:DC107)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="108" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>223</v>
       </c>
@@ -37180,15 +37180,15 @@
         <v>0</v>
       </c>
       <c r="DD108">
-        <f>SUM(D108:DC108)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="DE108" s="1">
-        <f>COUNT(D108:DC108)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>223</v>
       </c>
@@ -37511,15 +37511,15 @@
         <v>523</v>
       </c>
       <c r="DD109">
-        <f>SUM(D109:DC109)</f>
+        <f t="shared" si="6"/>
         <v>70488</v>
       </c>
       <c r="DE109" s="1">
-        <f>COUNT(D109:DC109)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="110" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>223</v>
       </c>
@@ -37842,15 +37842,15 @@
         <v>297</v>
       </c>
       <c r="DD110">
-        <f>SUM(D110:DC110)</f>
+        <f t="shared" si="6"/>
         <v>17723</v>
       </c>
       <c r="DE110" s="1">
-        <f>COUNT(D110:DC110)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="111" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>223</v>
       </c>
@@ -38173,15 +38173,15 @@
         <v>40</v>
       </c>
       <c r="DD111">
-        <f>SUM(D111:DC111)</f>
+        <f t="shared" si="6"/>
         <v>82979</v>
       </c>
       <c r="DE111" s="1">
-        <f>COUNT(D111:DC111)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="112" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>223</v>
       </c>
@@ -38504,15 +38504,15 @@
         <v>4126</v>
       </c>
       <c r="DD112">
-        <f>SUM(D112:DC112)</f>
+        <f t="shared" si="6"/>
         <v>740827</v>
       </c>
       <c r="DE112" s="1">
-        <f>COUNT(D112:DC112)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="113" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>223</v>
       </c>
@@ -38835,15 +38835,15 @@
         <v>0</v>
       </c>
       <c r="DD113">
-        <f>SUM(D113:DC113)</f>
+        <f t="shared" si="6"/>
         <v>55</v>
       </c>
       <c r="DE113" s="1">
-        <f>COUNT(D113:DC113)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="114" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>223</v>
       </c>
@@ -39166,15 +39166,15 @@
         <v>349</v>
       </c>
       <c r="DD114">
-        <f>SUM(D114:DC114)</f>
+        <f t="shared" si="6"/>
         <v>76777</v>
       </c>
       <c r="DE114" s="1">
-        <f>COUNT(D114:DC114)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="115" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>244</v>
       </c>
@@ -39497,15 +39497,15 @@
         <v>270</v>
       </c>
       <c r="DD115">
-        <f>SUM(D115:DC115)</f>
+        <f t="shared" si="6"/>
         <v>140429</v>
       </c>
       <c r="DE115" s="1">
-        <f>COUNT(D115:DC115)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="116" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>244</v>
       </c>
@@ -39828,15 +39828,15 @@
         <v>111</v>
       </c>
       <c r="DD116">
-        <f>SUM(D116:DC116)</f>
+        <f t="shared" si="6"/>
         <v>42709</v>
       </c>
       <c r="DE116" s="1">
-        <f>COUNT(D116:DC116)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="117" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>244</v>
       </c>
@@ -40159,15 +40159,15 @@
         <v>1029</v>
       </c>
       <c r="DD117">
-        <f>SUM(D117:DC117)</f>
+        <f t="shared" si="6"/>
         <v>237076</v>
       </c>
       <c r="DE117" s="1">
-        <f>COUNT(D117:DC117)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="118" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>244</v>
       </c>
@@ -40490,15 +40490,15 @@
         <v>344</v>
       </c>
       <c r="DD118">
-        <f>SUM(D118:DC118)</f>
+        <f t="shared" si="6"/>
         <v>217287</v>
       </c>
       <c r="DE118" s="1">
-        <f>COUNT(D118:DC118)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="119" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>244</v>
       </c>
@@ -40821,15 +40821,15 @@
         <v>121</v>
       </c>
       <c r="DD119">
-        <f>SUM(D119:DC119)</f>
+        <f t="shared" si="6"/>
         <v>41845</v>
       </c>
       <c r="DE119" s="1">
-        <f>COUNT(D119:DC119)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="120" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>244</v>
       </c>
@@ -41152,15 +41152,15 @@
         <v>70</v>
       </c>
       <c r="DD120">
-        <f>SUM(D120:DC120)</f>
+        <f t="shared" si="6"/>
         <v>58567</v>
       </c>
       <c r="DE120" s="1">
-        <f>COUNT(D120:DC120)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="121" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>244</v>
       </c>
@@ -41483,15 +41483,15 @@
         <v>25</v>
       </c>
       <c r="DD121">
-        <f>SUM(D121:DC121)</f>
+        <f t="shared" si="6"/>
         <v>3032</v>
       </c>
       <c r="DE121" s="1">
-        <f>COUNT(D121:DC121)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="122" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>244</v>
       </c>
@@ -41814,15 +41814,15 @@
         <v>38</v>
       </c>
       <c r="DD122">
-        <f>SUM(D122:DC122)</f>
+        <f t="shared" si="6"/>
         <v>21015</v>
       </c>
       <c r="DE122" s="1">
-        <f>COUNT(D122:DC122)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="123" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>244</v>
       </c>
@@ -42145,15 +42145,15 @@
         <v>457</v>
       </c>
       <c r="DD123">
-        <f>SUM(D123:DC123)</f>
+        <f t="shared" si="6"/>
         <v>66055</v>
       </c>
       <c r="DE123" s="1">
-        <f>COUNT(D123:DC123)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="124" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>244</v>
       </c>
@@ -42476,15 +42476,15 @@
         <v>374</v>
       </c>
       <c r="DD124">
-        <f>SUM(D124:DC124)</f>
+        <f t="shared" si="6"/>
         <v>77750</v>
       </c>
       <c r="DE124" s="1">
-        <f>COUNT(D124:DC124)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="125" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>244</v>
       </c>
@@ -42807,15 +42807,15 @@
         <v>263</v>
       </c>
       <c r="DD125">
-        <f>SUM(D125:DC125)</f>
+        <f t="shared" si="6"/>
         <v>64477</v>
       </c>
       <c r="DE125" s="1">
-        <f>COUNT(D125:DC125)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="126" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>244</v>
       </c>
@@ -43138,15 +43138,15 @@
         <v>846</v>
       </c>
       <c r="DD126">
-        <f>SUM(D126:DC126)</f>
+        <f t="shared" si="6"/>
         <v>214223</v>
       </c>
       <c r="DE126" s="1">
-        <f>COUNT(D126:DC126)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="127" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>244</v>
       </c>
@@ -43469,15 +43469,15 @@
         <v>1113</v>
       </c>
       <c r="DD127">
-        <f>SUM(D127:DC127)</f>
+        <f t="shared" si="6"/>
         <v>209107</v>
       </c>
       <c r="DE127" s="1">
-        <f>COUNT(D127:DC127)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="128" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>244</v>
       </c>
@@ -43800,15 +43800,15 @@
         <v>889</v>
       </c>
       <c r="DD128">
-        <f>SUM(D128:DC128)</f>
+        <f t="shared" si="6"/>
         <v>173458</v>
       </c>
       <c r="DE128" s="1">
-        <f>COUNT(D128:DC128)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="129" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>244</v>
       </c>
@@ -44131,15 +44131,15 @@
         <v>50</v>
       </c>
       <c r="DD129">
-        <f>SUM(D129:DC129)</f>
+        <f t="shared" si="6"/>
         <v>2653</v>
       </c>
       <c r="DE129" s="1">
-        <f>COUNT(D129:DC129)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="130" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>270</v>
       </c>
@@ -44462,15 +44462,15 @@
         <v>20</v>
       </c>
       <c r="DD130">
-        <f>SUM(D130:DC130)</f>
+        <f t="shared" si="6"/>
         <v>5710</v>
       </c>
       <c r="DE130" s="1">
-        <f>COUNT(D130:DC130)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="131" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>270</v>
       </c>
@@ -44793,15 +44793,15 @@
         <v>1316</v>
       </c>
       <c r="DD131">
-        <f>SUM(D131:DC131)</f>
+        <f t="shared" si="6"/>
         <v>262371</v>
       </c>
       <c r="DE131" s="1">
-        <f>COUNT(D131:DC131)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="132" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>270</v>
       </c>
@@ -45124,15 +45124,15 @@
         <v>1779</v>
       </c>
       <c r="DD132">
-        <f>SUM(D132:DC132)</f>
+        <f t="shared" si="6"/>
         <v>459795</v>
       </c>
       <c r="DE132" s="1">
-        <f>COUNT(D132:DC132)</f>
+        <f t="shared" si="7"/>
         <v>104</v>
       </c>
     </row>
-    <row r="133" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>270</v>
       </c>
@@ -45455,15 +45455,15 @@
         <v>107</v>
       </c>
       <c r="DD133">
-        <f>SUM(D133:DC133)</f>
+        <f t="shared" ref="DD133:DD164" si="8">SUM(D133:DC133)</f>
         <v>26016</v>
       </c>
       <c r="DE133" s="1">
-        <f>COUNT(D133:DC133)</f>
+        <f t="shared" ref="DE133:DE165" si="9">COUNT(D133:DC133)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="134" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>270</v>
       </c>
@@ -45786,15 +45786,15 @@
         <v>4336</v>
       </c>
       <c r="DD134">
-        <f>SUM(D134:DC134)</f>
+        <f t="shared" si="8"/>
         <v>951406</v>
       </c>
       <c r="DE134" s="1">
-        <f>COUNT(D134:DC134)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="135" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>270</v>
       </c>
@@ -46117,15 +46117,15 @@
         <v>547</v>
       </c>
       <c r="DD135">
-        <f>SUM(D135:DC135)</f>
+        <f t="shared" si="8"/>
         <v>208138</v>
       </c>
       <c r="DE135" s="1">
-        <f>COUNT(D135:DC135)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="136" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>270</v>
       </c>
@@ -46448,15 +46448,15 @@
         <v>163</v>
       </c>
       <c r="DD136">
-        <f>SUM(D136:DC136)</f>
+        <f t="shared" si="8"/>
         <v>44676</v>
       </c>
       <c r="DE136" s="1">
-        <f>COUNT(D136:DC136)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="137" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>270</v>
       </c>
@@ -46779,15 +46779,15 @@
         <v>10284</v>
       </c>
       <c r="DD137">
-        <f>SUM(D137:DC137)</f>
+        <f t="shared" si="8"/>
         <v>1283054</v>
       </c>
       <c r="DE137" s="1">
-        <f>COUNT(D137:DC137)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="138" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>270</v>
       </c>
@@ -47110,15 +47110,15 @@
         <v>82</v>
       </c>
       <c r="DD138">
-        <f>SUM(D138:DC138)</f>
+        <f t="shared" si="8"/>
         <v>40996</v>
       </c>
       <c r="DE138" s="1">
-        <f>COUNT(D138:DC138)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="139" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>270</v>
       </c>
@@ -47441,15 +47441,15 @@
         <v>67</v>
       </c>
       <c r="DD139">
-        <f>SUM(D139:DC139)</f>
+        <f t="shared" si="8"/>
         <v>20124</v>
       </c>
       <c r="DE139" s="1">
-        <f>COUNT(D139:DC139)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="140" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>270</v>
       </c>
@@ -47772,15 +47772,15 @@
         <v>0</v>
       </c>
       <c r="DD140">
-        <f>SUM(D140:DC140)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="DE140" s="1">
-        <f>COUNT(D140:DC140)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="141" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>285</v>
       </c>
@@ -48103,15 +48103,15 @@
         <v>528</v>
       </c>
       <c r="DD141">
-        <f>SUM(D141:DC141)</f>
+        <f t="shared" si="8"/>
         <v>123385</v>
       </c>
       <c r="DE141" s="1">
-        <f>COUNT(D141:DC141)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="142" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>285</v>
       </c>
@@ -48434,15 +48434,15 @@
         <v>5171</v>
       </c>
       <c r="DD142">
-        <f>SUM(D142:DC142)</f>
+        <f t="shared" si="8"/>
         <v>1183413</v>
       </c>
       <c r="DE142" s="1">
-        <f>COUNT(D142:DC142)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="143" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>284</v>
       </c>
@@ -48765,15 +48765,15 @@
         <v>1325</v>
       </c>
       <c r="DD143">
-        <f>SUM(D143:DC143)</f>
+        <f t="shared" si="8"/>
         <v>418002</v>
       </c>
       <c r="DE143" s="1">
-        <f>COUNT(D143:DC143)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="144" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>284</v>
       </c>
@@ -49096,15 +49096,15 @@
         <v>0</v>
       </c>
       <c r="DD144">
-        <f>SUM(D144:DC144)</f>
+        <f t="shared" si="8"/>
         <v>3939</v>
       </c>
       <c r="DE144" s="1">
-        <f>COUNT(D144:DC144)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="145" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>284</v>
       </c>
@@ -49427,15 +49427,15 @@
         <v>84</v>
       </c>
       <c r="DD145">
-        <f>SUM(D145:DC145)</f>
+        <f t="shared" si="8"/>
         <v>17925</v>
       </c>
       <c r="DE145" s="1">
-        <f>COUNT(D145:DC145)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="146" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>284</v>
       </c>
@@ -49758,15 +49758,15 @@
         <v>1282</v>
       </c>
       <c r="DD146">
-        <f>SUM(D146:DC146)</f>
+        <f t="shared" si="8"/>
         <v>454419</v>
       </c>
       <c r="DE146" s="1">
-        <f>COUNT(D146:DC146)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="147" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>284</v>
       </c>
@@ -50089,15 +50089,15 @@
         <v>5</v>
       </c>
       <c r="DD147">
-        <f>SUM(D147:DC147)</f>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="DE147" s="1">
-        <f>COUNT(D147:DC147)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="148" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>304</v>
       </c>
@@ -50420,15 +50420,15 @@
         <v>224</v>
       </c>
       <c r="DD148">
-        <f>SUM(D148:DC148)</f>
+        <f t="shared" si="8"/>
         <v>64597</v>
       </c>
       <c r="DE148" s="1">
-        <f>COUNT(D148:DC148)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="149" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>304</v>
       </c>
@@ -50751,15 +50751,15 @@
         <v>0</v>
       </c>
       <c r="DD149">
-        <f>SUM(D149:DC149)</f>
+        <f t="shared" si="8"/>
         <v>28446</v>
       </c>
       <c r="DE149" s="1">
-        <f>COUNT(D149:DC149)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="150" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>304</v>
       </c>
@@ -51082,15 +51082,15 @@
         <v>130</v>
       </c>
       <c r="DD150">
-        <f>SUM(D150:DC150)</f>
+        <f t="shared" si="8"/>
         <v>26452</v>
       </c>
       <c r="DE150" s="1">
-        <f>COUNT(D150:DC150)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="151" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>304</v>
       </c>
@@ -51413,15 +51413,15 @@
         <v>384</v>
       </c>
       <c r="DD151">
-        <f>SUM(D151:DC151)</f>
+        <f t="shared" si="8"/>
         <v>85051</v>
       </c>
       <c r="DE151" s="1">
-        <f>COUNT(D151:DC151)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="152" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>304</v>
       </c>
@@ -51744,15 +51744,15 @@
         <v>0</v>
       </c>
       <c r="DD152">
-        <f>SUM(D152:DC152)</f>
+        <f t="shared" si="8"/>
         <v>332</v>
       </c>
       <c r="DE152" s="1">
-        <f>COUNT(D152:DC152)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="153" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>304</v>
       </c>
@@ -52075,15 +52075,15 @@
         <v>0</v>
       </c>
       <c r="DD153">
-        <f>SUM(D153:DC153)</f>
+        <f t="shared" si="8"/>
         <v>807</v>
       </c>
       <c r="DE153" s="1">
-        <f>COUNT(D153:DC153)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="154" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>260</v>
       </c>
@@ -52406,15 +52406,15 @@
         <v>0</v>
       </c>
       <c r="DD154">
-        <f>SUM(D154:DC154)</f>
+        <f t="shared" si="8"/>
         <v>34</v>
       </c>
       <c r="DE154" s="1">
-        <f>COUNT(D154:DC154)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="155" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>260</v>
       </c>
@@ -52737,15 +52737,15 @@
         <v>0</v>
       </c>
       <c r="DD155">
-        <f>SUM(D155:DC155)</f>
+        <f t="shared" si="8"/>
         <v>210</v>
       </c>
       <c r="DE155" s="1">
-        <f>COUNT(D155:DC155)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="156" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>260</v>
       </c>
@@ -53068,15 +53068,15 @@
         <v>178</v>
       </c>
       <c r="DD156">
-        <f>SUM(D156:DC156)</f>
+        <f t="shared" si="8"/>
         <v>48373</v>
       </c>
       <c r="DE156" s="1">
-        <f>COUNT(D156:DC156)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="157" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>260</v>
       </c>
@@ -53399,15 +53399,15 @@
         <v>2777</v>
       </c>
       <c r="DD157">
-        <f>SUM(D157:DC157)</f>
+        <f t="shared" si="8"/>
         <v>530186</v>
       </c>
       <c r="DE157" s="1">
-        <f>COUNT(D157:DC157)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="158" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>260</v>
       </c>
@@ -53730,15 +53730,15 @@
         <v>38</v>
       </c>
       <c r="DD158">
-        <f>SUM(D158:DC158)</f>
+        <f t="shared" si="8"/>
         <v>41471</v>
       </c>
       <c r="DE158" s="1">
-        <f>COUNT(D158:DC158)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="159" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>260</v>
       </c>
@@ -54061,15 +54061,15 @@
         <v>0</v>
       </c>
       <c r="DD159">
-        <f>SUM(D159:DC159)</f>
+        <f t="shared" si="8"/>
         <v>55</v>
       </c>
       <c r="DE159" s="1">
-        <f>COUNT(D159:DC159)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="160" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>260</v>
       </c>
@@ -54392,15 +54392,15 @@
         <v>0</v>
       </c>
       <c r="DD160">
-        <f>SUM(D160:DC160)</f>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="DE160" s="1">
-        <f>COUNT(D160:DC160)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="161" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>260</v>
       </c>
@@ -54723,15 +54723,15 @@
         <v>1</v>
       </c>
       <c r="DD161">
-        <f>SUM(D161:DC161)</f>
+        <f t="shared" si="8"/>
         <v>7400</v>
       </c>
       <c r="DE161" s="1">
-        <f>COUNT(D161:DC161)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="162" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>260</v>
       </c>
@@ -55054,15 +55054,15 @@
         <v>3157</v>
       </c>
       <c r="DD162">
-        <f>SUM(D162:DC162)</f>
+        <f t="shared" si="8"/>
         <v>407424</v>
       </c>
       <c r="DE162" s="1">
-        <f>COUNT(D162:DC162)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="163" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>260</v>
       </c>
@@ -55385,15 +55385,15 @@
         <v>8928</v>
       </c>
       <c r="DD163">
-        <f>SUM(D163:DC163)</f>
+        <f t="shared" si="8"/>
         <v>907397</v>
       </c>
       <c r="DE163" s="1">
-        <f>COUNT(D163:DC163)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="164" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>328</v>
       </c>
@@ -55716,15 +55716,15 @@
         <v>42975</v>
       </c>
       <c r="DD164">
-        <f>SUM(D164:DC164)</f>
+        <f t="shared" si="8"/>
         <v>2059879</v>
       </c>
       <c r="DE164" s="1">
-        <f>COUNT(D164:DC164)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
-    <row r="165" spans="1:109" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>328</v>
       </c>
@@ -56047,11 +56047,11 @@
         <v>357234</v>
       </c>
       <c r="DD165">
-        <f>SUM(D165:DC165)</f>
+        <f t="shared" ref="DD165:DD196" si="10">SUM(D165:DC165)</f>
         <v>56379711</v>
       </c>
       <c r="DE165" s="1">
-        <f>COUNT(D165:DC165)</f>
+        <f t="shared" si="9"/>
         <v>104</v>
       </c>
     </row>
@@ -56065,24 +56065,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DG28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="5" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="109" width="8.7265625" style="1"/>
-    <col min="111" max="111" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="109" width="8.7109375" style="1"/>
+    <col min="111" max="111" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:111" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>331</v>
       </c>
@@ -56396,7 +56396,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="2" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:111" x14ac:dyDescent="0.25">
       <c r="F2" s="1">
         <v>2014</v>
       </c>
@@ -56710,7 +56710,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:111" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:111" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>435</v>
       </c>
@@ -57045,7 +57045,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>54</v>
       </c>
@@ -57377,11 +57377,11 @@
         <v>29931</v>
       </c>
       <c r="DG4" s="5">
-        <f>COUNT(F4:DE4)</f>
+        <f t="shared" ref="DG4:DG28" si="0">COUNT(F4:DE4)</f>
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>54</v>
       </c>
@@ -57713,11 +57713,11 @@
         <v>24625</v>
       </c>
       <c r="DG5" s="5">
-        <f>COUNT(F5:DE5)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -58049,11 +58049,11 @@
         <v>123157</v>
       </c>
       <c r="DG6" s="5">
-        <f>COUNT(F6:DE6)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="7" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>77</v>
       </c>
@@ -58385,11 +58385,11 @@
         <v>428705</v>
       </c>
       <c r="DG7" s="5">
-        <f>COUNT(F7:DE7)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>95</v>
       </c>
@@ -58721,11 +58721,11 @@
         <v>1225467</v>
       </c>
       <c r="DG8" s="5">
-        <f>COUNT(F8:DE8)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>104</v>
       </c>
@@ -59057,11 +59057,11 @@
         <v>868741</v>
       </c>
       <c r="DG9" s="5">
-        <f>COUNT(F9:DE9)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>110</v>
       </c>
@@ -59393,11 +59393,11 @@
         <v>74446</v>
       </c>
       <c r="DG10" s="5">
-        <f>COUNT(F10:DE10)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>123</v>
       </c>
@@ -59729,11 +59729,11 @@
         <v>16074</v>
       </c>
       <c r="DG11" s="5">
-        <f>COUNT(F11:DE11)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>142</v>
       </c>
@@ -60065,11 +60065,11 @@
         <v>21359</v>
       </c>
       <c r="DG12" s="5">
-        <f>COUNT(F12:DE12)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="13" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>142</v>
       </c>
@@ -60401,11 +60401,11 @@
         <v>34857</v>
       </c>
       <c r="DG13" s="5">
-        <f>COUNT(F13:DE13)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>160</v>
       </c>
@@ -60737,11 +60737,11 @@
         <v>70718</v>
       </c>
       <c r="DG14" s="5">
-        <f>COUNT(F14:DE14)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>160</v>
       </c>
@@ -61073,11 +61073,11 @@
         <v>1040</v>
       </c>
       <c r="DG15" s="5">
-        <f>COUNT(F15:DE15)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>175</v>
       </c>
@@ -61409,11 +61409,11 @@
         <v>8648</v>
       </c>
       <c r="DG16" s="5">
-        <f>COUNT(F16:DE16)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>223</v>
       </c>
@@ -61745,11 +61745,11 @@
         <v>59848</v>
       </c>
       <c r="DG17" s="5">
-        <f>COUNT(F17:DE17)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>244</v>
       </c>
@@ -62081,11 +62081,11 @@
         <v>14050</v>
       </c>
       <c r="DG18" s="5">
-        <f>COUNT(F18:DE18)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>244</v>
       </c>
@@ -62417,11 +62417,11 @@
         <v>5426</v>
       </c>
       <c r="DG19" s="5">
-        <f>COUNT(F19:DE19)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>270</v>
       </c>
@@ -62753,11 +62753,11 @@
         <v>13546</v>
       </c>
       <c r="DG20" s="5">
-        <f>COUNT(F20:DE20)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>270</v>
       </c>
@@ -63089,11 +63089,11 @@
         <v>16700</v>
       </c>
       <c r="DG21" s="5">
-        <f>COUNT(F21:DE21)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>270</v>
       </c>
@@ -63425,11 +63425,11 @@
         <v>18870</v>
       </c>
       <c r="DG22" s="5">
-        <f>COUNT(F22:DE22)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>285</v>
       </c>
@@ -63761,11 +63761,11 @@
         <v>29484</v>
       </c>
       <c r="DG23" s="5">
-        <f>COUNT(F23:DE23)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>284</v>
       </c>
@@ -64097,11 +64097,11 @@
         <v>14850</v>
       </c>
       <c r="DG24" s="5">
-        <f>COUNT(F24:DE24)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="25" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>284</v>
       </c>
@@ -64433,11 +64433,11 @@
         <v>14007</v>
       </c>
       <c r="DG25" s="5">
-        <f>COUNT(F25:DE25)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>260</v>
       </c>
@@ -64769,11 +64769,11 @@
         <v>36471</v>
       </c>
       <c r="DG26" s="5">
-        <f>COUNT(F26:DE26)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>260</v>
       </c>
@@ -65105,11 +65105,11 @@
         <v>17044</v>
       </c>
       <c r="DG27" s="5">
-        <f>COUNT(F27:DE27)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:111" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>260</v>
       </c>
@@ -65441,7 +65441,7 @@
         <v>49068</v>
       </c>
       <c r="DG28" s="5">
-        <f>COUNT(F28:DE28)</f>
+        <f t="shared" si="0"/>
         <v>104</v>
       </c>
     </row>
@@ -65455,24 +65455,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CP30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="3" topLeftCell="AL4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="92" width="8.7265625" style="1"/>
-    <col min="94" max="94" width="8.7265625" style="1"/>
+    <col min="1" max="1" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="92" width="8.7109375" style="1"/>
+    <col min="94" max="94" width="8.7109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:94" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:94" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>331</v>
       </c>
@@ -65735,7 +65735,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:94" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:94" x14ac:dyDescent="0.25">
       <c r="F2" s="1">
         <v>2014</v>
       </c>
@@ -65998,7 +65998,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="3" spans="1:94" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>435</v>
       </c>
@@ -66282,7 +66282,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>54</v>
       </c>
@@ -66563,11 +66563,11 @@
         <v>16973</v>
       </c>
       <c r="CP4" s="7">
-        <f>COUNT(F4:CN4)</f>
+        <f t="shared" ref="CP4:CP30" si="0">COUNT(F4:CN4)</f>
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>54</v>
       </c>
@@ -66848,11 +66848,11 @@
         <v>15737</v>
       </c>
       <c r="CP5" s="7">
-        <f>COUNT(F5:CN5)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>54</v>
       </c>
@@ -67133,11 +67133,11 @@
         <v>16555</v>
       </c>
       <c r="CP6" s="7">
-        <f>COUNT(F6:CN6)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>54</v>
       </c>
@@ -67418,11 +67418,11 @@
         <v>17685</v>
       </c>
       <c r="CP7" s="7">
-        <f>COUNT(F7:CN7)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>54</v>
       </c>
@@ -67703,11 +67703,11 @@
         <v>92007</v>
       </c>
       <c r="CP8" s="7">
-        <f>COUNT(F8:CN8)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>77</v>
       </c>
@@ -67988,11 +67988,11 @@
         <v>8008</v>
       </c>
       <c r="CP9" s="7">
-        <f>COUNT(F9:CN9)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>77</v>
       </c>
@@ -68273,11 +68273,11 @@
         <v>9568</v>
       </c>
       <c r="CP10" s="7">
-        <f>COUNT(F10:CN10)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>95</v>
       </c>
@@ -68558,11 +68558,11 @@
         <v>495393</v>
       </c>
       <c r="CP11" s="7">
-        <f>COUNT(F11:CN11)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="12" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>104</v>
       </c>
@@ -68843,11 +68843,11 @@
         <v>128431</v>
       </c>
       <c r="CP12" s="7">
-        <f>COUNT(F12:CN12)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>110</v>
       </c>
@@ -69128,11 +69128,11 @@
         <v>15611</v>
       </c>
       <c r="CP13" s="7">
-        <f>COUNT(F13:CN13)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="14" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>123</v>
       </c>
@@ -69413,11 +69413,11 @@
         <v>34788</v>
       </c>
       <c r="CP14" s="7">
-        <f>COUNT(F14:CN14)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>123</v>
       </c>
@@ -69698,11 +69698,11 @@
         <v>29961</v>
       </c>
       <c r="CP15" s="7">
-        <f>COUNT(F15:CN15)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="16" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>142</v>
       </c>
@@ -69983,11 +69983,11 @@
         <v>38537</v>
       </c>
       <c r="CP16" s="7">
-        <f>COUNT(F16:CN16)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>142</v>
       </c>
@@ -70268,11 +70268,11 @@
         <v>57572</v>
       </c>
       <c r="CP17" s="7">
-        <f>COUNT(F17:CN17)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="18" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>160</v>
       </c>
@@ -70553,11 +70553,11 @@
         <v>20844</v>
       </c>
       <c r="CP18" s="7">
-        <f>COUNT(F18:CN18)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>160</v>
       </c>
@@ -70838,11 +70838,11 @@
         <v>30715</v>
       </c>
       <c r="CP19" s="7">
-        <f>COUNT(F19:CN19)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>160</v>
       </c>
@@ -71123,11 +71123,11 @@
         <v>162800</v>
       </c>
       <c r="CP20" s="7">
-        <f>COUNT(F20:CN20)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>175</v>
       </c>
@@ -71408,11 +71408,11 @@
         <v>15132</v>
       </c>
       <c r="CP21" s="7">
-        <f>COUNT(F21:CN21)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>175</v>
       </c>
@@ -71693,11 +71693,11 @@
         <v>15635</v>
       </c>
       <c r="CP22" s="7">
-        <f>COUNT(F22:CN22)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>244</v>
       </c>
@@ -71978,11 +71978,11 @@
         <v>5901</v>
       </c>
       <c r="CP23" s="7">
-        <f>COUNT(F23:CN23)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>244</v>
       </c>
@@ -72263,11 +72263,11 @@
         <v>37373</v>
       </c>
       <c r="CP24" s="7">
-        <f>COUNT(F24:CN24)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="25" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>270</v>
       </c>
@@ -72548,11 +72548,11 @@
         <v>66138</v>
       </c>
       <c r="CP25" s="7">
-        <f>COUNT(F25:CN25)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>270</v>
       </c>
@@ -72833,11 +72833,11 @@
         <v>30740</v>
       </c>
       <c r="CP26" s="7">
-        <f>COUNT(F26:CN26)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
         <v>285</v>
       </c>
@@ -73118,11 +73118,11 @@
         <v>33679</v>
       </c>
       <c r="CP27" s="7">
-        <f>COUNT(F27:CN27)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>284</v>
       </c>
@@ -73403,11 +73403,11 @@
         <v>14000</v>
       </c>
       <c r="CP28" s="7">
-        <f>COUNT(F28:CN28)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>284</v>
       </c>
@@ -73688,11 +73688,11 @@
         <v>15625</v>
       </c>
       <c r="CP29" s="7">
-        <f>COUNT(F29:CN29)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:94" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>260</v>
       </c>
@@ -73973,7 +73973,7 @@
         <v>7280</v>
       </c>
       <c r="CP30" s="7">
-        <f>COUNT(F30:CN30)</f>
+        <f t="shared" si="0"/>
         <v>87</v>
       </c>
     </row>

</xml_diff>